<commit_message>
Search and store in Arraylist Success
</commit_message>
<xml_diff>
--- a/testData/testdata.xlsx
+++ b/testData/testdata.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yamah022\Desktop\javra\workspace\automation_project\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yamah022\Desktop\javra\selenium-workspace\proponent\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="caseNo" sheetId="3" r:id="rId2"/>
+    <sheet name="customerNo" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>browser</t>
   </si>
@@ -48,13 +50,22 @@
   </si>
   <si>
     <t>chrome</t>
+  </si>
+  <si>
+    <t>case numbers to be searched</t>
+  </si>
+  <si>
+    <t>Customer number search data</t>
+  </si>
+  <si>
+    <t>P36355</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,16 +81,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,14 +116,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -378,7 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -426,4 +482,81 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>7931588</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>119067</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>122743</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>3065</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>82469</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>